<commit_message>
feat: Màn hình tải danh sách Đối kháng, Đơn luyện, song luyện, đa luyện, tự vệ,.. tính điểm Đối kháng
</commit_message>
<xml_diff>
--- a/VHD-SCOREBOARD-TEMPLATE-SAMPLE.xlsx
+++ b/VHD-SCOREBOARD-TEMPLATE-SAMPLE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/feliz/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/feliz/Documents/binhtanICT/scoreboard-ict/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA16D22-00AD-BE4D-A41E-9E032BB074ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727950B1-7C48-494C-87D7-E61D1FBDE196}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="39580" windowHeight="25100" activeTab="8" xr2:uid="{4B7BE7C1-6C83-1244-AA26-03E3488ECB8E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="39580" windowHeight="25100" activeTab="3" xr2:uid="{4B7BE7C1-6C83-1244-AA26-03E3488ECB8E}"/>
   </bookViews>
   <sheets>
     <sheet name="DK-Nhóm 1" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1869" uniqueCount="174">
   <si>
     <t>Họ tên</t>
   </si>
@@ -7072,8 +7072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E11D123C-A42C-9C44-9BDF-8952717AE253}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7485,7 +7485,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="A1:E9"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7533,15 +7533,11 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
-      <c r="B3" s="6" t="s">
-        <v>170</v>
-      </c>
+      <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -7563,15 +7559,11 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
-      <c r="B5" s="6" t="s">
-        <v>170</v>
-      </c>
+      <c r="B5" s="6"/>
       <c r="C5" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -7593,15 +7585,11 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
-      <c r="B7" s="6" t="s">
-        <v>170</v>
-      </c>
+      <c r="B7" s="6"/>
       <c r="C7" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -7623,15 +7611,11 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
-      <c r="B9" s="6" t="s">
-        <v>170</v>
-      </c>
+      <c r="B9" s="6"/>
       <c r="C9" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
   </sheetData>
@@ -7645,7 +7629,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="A1:E9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7689,15 +7673,11 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
-      <c r="B3" s="6" t="s">
-        <v>147</v>
-      </c>
+      <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -7719,15 +7699,11 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
-      <c r="B5" s="6" t="s">
-        <v>147</v>
-      </c>
+      <c r="B5" s="6"/>
       <c r="C5" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -7749,15 +7725,11 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
-      <c r="B7" s="6" t="s">
-        <v>147</v>
-      </c>
+      <c r="B7" s="6"/>
       <c r="C7" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -7779,15 +7751,11 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
-      <c r="B9" s="6" t="s">
-        <v>147</v>
-      </c>
+      <c r="B9" s="6"/>
       <c r="C9" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
   </sheetData>
@@ -7943,7 +7911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AA3EC8-2059-9549-8D6E-F3258D6A2FF1}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="282" workbookViewId="0">
+    <sheetView zoomScale="282" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>

</xml_diff>